<commit_message>
Exercício 1 - Spreadsheet de compressão
</commit_message>
<xml_diff>
--- a/ex1/compression.xlsx
+++ b/ex1/compression.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universidadedecoimbra154-my.sharepoint.com/personal/uc2019218299_student_uc_pt/Documents/Year 3/2nd Semester/Mult/PLs/tp1/ex1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="125" documentId="11_AD4DF034E34935FBC521DCAAF71F48E25ADEDD8B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{929A730B-201B-4482-90FC-C09371438875}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="11_AD4DF034E34935FBC521DCAAF71F48E25ADEDD8B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{775FE0F1-EB22-4D3D-BD56-013016BE1AE8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,18 +36,27 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="13">
   <si>
+    <t>barn.bmp</t>
+  </si>
+  <si>
+    <t>quality</t>
+  </si>
+  <si>
+    <t>size</t>
+  </si>
+  <si>
+    <t>original</t>
+  </si>
+  <si>
+    <t>barn</t>
+  </si>
+  <si>
+    <t>logo</t>
+  </si>
+  <si>
     <t>peppers</t>
   </si>
   <si>
-    <t>quality</t>
-  </si>
-  <si>
-    <t>size</t>
-  </si>
-  <si>
-    <t>original</t>
-  </si>
-  <si>
     <t>high</t>
   </si>
   <si>
@@ -58,22 +66,13 @@
     <t>low</t>
   </si>
   <si>
-    <t>barn</t>
-  </si>
-  <si>
-    <t>logo</t>
-  </si>
-  <si>
-    <t>barn.bmp</t>
-  </si>
-  <si>
     <t>logo.bmp</t>
   </si>
   <si>
     <t>peppers.bmp</t>
   </si>
   <si>
-    <t>Compression ratios.bmp</t>
+    <t>Compression ratios</t>
   </si>
 </sst>
 </file>
@@ -128,24 +127,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -292,68 +287,68 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D00929E2-2F95-4404-BDE6-4D65F14903A6}" name="peppers" displayName="peppers" ref="B3:C7" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D00929E2-2F95-4404-BDE6-4D65F14903A6}" name="peppers" displayName="peppers" ref="B3:C7" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="B3:C7" xr:uid="{D00929E2-2F95-4404-BDE6-4D65F14903A6}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3A9121D3-7651-4CBA-ADA3-F7F2E16D1C18}" name="quality" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{DE680829-A686-4CC8-AA2D-91416D5E8C44}" name="size" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{3A9121D3-7651-4CBA-ADA3-F7F2E16D1C18}" name="quality" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{DE680829-A686-4CC8-AA2D-91416D5E8C44}" name="size" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5A51F1C8-7C95-4BD3-97F0-8D9DB1C62DB9}" name="peppers4" displayName="peppers4" ref="B10:C14" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{5A51F1C8-7C95-4BD3-97F0-8D9DB1C62DB9}" name="peppers4" displayName="peppers4" ref="B10:C14" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="B10:C14" xr:uid="{5A51F1C8-7C95-4BD3-97F0-8D9DB1C62DB9}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{DC2DA71B-30A1-4143-852D-263C88E1CDFB}" name="quality" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{707D0B6A-5FD6-4E90-8DD5-C607A7EB0E0C}" name="size" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{DC2DA71B-30A1-4143-852D-263C88E1CDFB}" name="quality" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{707D0B6A-5FD6-4E90-8DD5-C607A7EB0E0C}" name="size" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4D2ACBF9-FA44-40B1-BF51-B326351D2ABB}" name="peppers5" displayName="peppers5" ref="B17:C21" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{4D2ACBF9-FA44-40B1-BF51-B326351D2ABB}" name="peppers5" displayName="peppers5" ref="B17:C21" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
   <autoFilter ref="B17:C21" xr:uid="{4D2ACBF9-FA44-40B1-BF51-B326351D2ABB}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{D2B4C1F1-EDD4-47E3-8FA5-7D2B8F5FF5F2}" name="quality" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{C7B84EE4-35E4-40AB-B7BE-2DA695FF43B9}" name="size" dataDxfId="10"/>
+    <tableColumn id="1" xr3:uid="{D2B4C1F1-EDD4-47E3-8FA5-7D2B8F5FF5F2}" name="quality" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{C7B84EE4-35E4-40AB-B7BE-2DA695FF43B9}" name="size" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AE4BE0FF-0986-4B84-B813-C349C4F4A888}" name="Tabela5" displayName="Tabela5" ref="E4:H7" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="E4:H7" xr:uid="{AE4BE0FF-0986-4B84-B813-C349C4F4A888}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AE4BE0FF-0986-4B84-B813-C349C4F4A888}" name="Tabela5" displayName="Tabela5" ref="E3:H6" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="E3:H6" xr:uid="{AE4BE0FF-0986-4B84-B813-C349C4F4A888}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
     <filterColumn colId="3" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{ADC3436B-3F4D-42E7-9416-8DD066D5698F}" name="quality" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{1EA6CCD8-1B52-44D8-892C-4A4449E752B4}" name="barn" dataDxfId="4">
+    <tableColumn id="1" xr3:uid="{ADC3436B-3F4D-42E7-9416-8DD066D5698F}" name="quality" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{1EA6CCD8-1B52-44D8-892C-4A4449E752B4}" name="barn" dataDxfId="2">
       <calculatedColumnFormula>ROUND($C$4/C5,0)&amp;":"&amp;1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{F934CF72-5BE4-4CD8-859F-E5C0C219F774}" name="logo" dataDxfId="3">
+    <tableColumn id="3" xr3:uid="{F934CF72-5BE4-4CD8-859F-E5C0C219F774}" name="logo" dataDxfId="1">
       <calculatedColumnFormula>ROUND($C$11/C12,0)&amp;":"&amp;1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{888F2343-6744-4719-AB34-95883565D659}" name="peppers" dataDxfId="2">
+    <tableColumn id="4" xr3:uid="{888F2343-6744-4719-AB34-95883565D659}" name="peppers" dataDxfId="0">
       <calculatedColumnFormula>ROUND($C$18/C19,0)&amp;":"&amp;1</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium20" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium20" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -620,10 +615,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:M21"/>
+  <dimension ref="B2:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,207 +628,204 @@
     <col min="8" max="8" width="10.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="E2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>356456</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="4" t="s">
+      <c r="E4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2">
-        <v>33859</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="5" t="str">
+      <c r="F4" s="3" t="str">
         <f>ROUND($C$4/C5,0)&amp;":"&amp;1</f>
         <v>11:1</v>
       </c>
-      <c r="G5" s="5" t="str">
+      <c r="G4" s="3" t="str">
         <f>ROUND($C$11/C12,0)&amp;":"&amp;1</f>
         <v>44:1</v>
       </c>
-      <c r="H5" s="5" t="str">
+      <c r="H4" s="3" t="str">
         <f>ROUND($C$18/C19,0)&amp;":"&amp;1</f>
         <v>19:1</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="1">
+        <v>33859</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="3" t="str">
+        <f>ROUND($C$4/C6,0)&amp;":"&amp;1</f>
+        <v>16:1</v>
+      </c>
+      <c r="G5" s="3" t="str">
+        <f>ROUND($C$11/C13,0)&amp;":"&amp;1</f>
+        <v>54:1</v>
+      </c>
+      <c r="H5" s="3" t="str">
+        <f>ROUND($C$18/C20,0)&amp;":"&amp;1</f>
+        <v>28:1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1">
         <v>22110</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" s="5" t="str">
-        <f t="shared" ref="F6:F7" si="0">ROUND($C$4/C6,0)&amp;":"&amp;1</f>
-        <v>16:1</v>
-      </c>
-      <c r="G6" s="5" t="str">
-        <f t="shared" ref="G6:G7" si="1">ROUND($C$11/C13,0)&amp;":"&amp;1</f>
-        <v>54:1</v>
-      </c>
-      <c r="H6" s="5" t="str">
-        <f t="shared" ref="H6:H7" si="2">ROUND($C$18/C20,0)&amp;":"&amp;1</f>
-        <v>28:1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="E6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="3" t="str">
+        <f>ROUND($C$4/C7,0)&amp;":"&amp;1</f>
+        <v>26:1</v>
+      </c>
+      <c r="G6" s="3" t="str">
+        <f>ROUND($C$11/C14,0)&amp;":"&amp;1</f>
+        <v>67:1</v>
+      </c>
+      <c r="H6" s="3" t="str">
+        <f>ROUND($C$18/C21,0)&amp;":"&amp;1</f>
+        <v>43:1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1">
         <v>13838</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v>26:1</v>
-      </c>
-      <c r="G7" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>67:1</v>
-      </c>
-      <c r="H7" s="5" t="str">
-        <f t="shared" si="2"/>
-        <v>43:1</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="M8" s="6"/>
-    </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B9" s="1" t="s">
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
+      <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>421556</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="2">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1">
         <v>9657</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="2">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="1">
         <v>7791</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14" s="2">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="1">
         <v>6333</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="1"/>
+      <c r="C16" s="4"/>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>589880</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="2">
+      <c r="B19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="1">
         <v>31326</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="2">
+      <c r="B20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1">
         <v>20797</v>
       </c>
     </row>
     <row r="21" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="2">
+      <c r="B21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="1">
         <v>13651</v>
       </c>
     </row>
@@ -842,7 +834,7 @@
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="E2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>